<commit_message>
corrected typo in reactions
</commit_message>
<xml_diff>
--- a/docs/examples/Literature data/Cupriavidus necator  Alagesan 2017/reactions.xlsx
+++ b/docs/examples/Literature data/Cupriavidus necator  Alagesan 2017/reactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krv114/Documents/GitHub/AutoFlow-OmicsDataHandling/docs/examples/Literature data/Cupriavidus necator  Alagesan 2017/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s143838/projects/AutoFlow-OmicsDataHandling/docs/examples/Literature data/Cupriavidus necator  Alagesan 2017/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6B94AC-CC41-2645-8B72-D08A0E5E6741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D41DC20-2BEC-6F4B-939E-B550167A5EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="500" windowWidth="10000" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9840" yWindow="500" windowWidth="22580" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -348,9 +348,6 @@
     <t>X5P (abcde) + R5P (fghij) -&gt; G3P (cde) + S7P (abfghij)</t>
   </si>
   <si>
-    <t>G3P (cde) + S7P (abfghhij) -&gt; X5P (abcde) + R5P (fghij)</t>
-  </si>
-  <si>
     <t>S7P (abcdefg) + G3P (hij) -&gt; E4P (defg) + F6P (abchij)</t>
   </si>
   <si>
@@ -475,6 +472,9 @@
   </si>
   <si>
     <t>PYR (abc) -&gt; PEP (abc)</t>
+  </si>
+  <si>
+    <t>G3P (cde) + S7P (abfghij) -&gt; X5P (abcde) + R5P (fghij)</t>
   </si>
 </sst>
 </file>
@@ -889,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -909,18 +909,18 @@
     </row>
     <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1000,7 +1000,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1144,7 +1144,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1232,7 +1232,7 @@
         <v>38</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1248,7 +1248,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1256,7 +1256,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
         <v>42</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>43</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>44</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1288,7 +1288,7 @@
         <v>45</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1296,7 +1296,7 @@
         <v>46</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
         <v>47</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
         <v>48</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1320,7 +1320,7 @@
         <v>49</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
         <v>50</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1336,7 +1336,7 @@
         <v>51</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
         <v>52</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1352,7 +1352,7 @@
         <v>53</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
         <v>54</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1368,7 +1368,7 @@
         <v>55</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1376,7 +1376,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
         <v>59</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>60</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>61</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>64</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>65</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
         <v>66</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>67</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>68</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>69</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>70</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1496,7 +1496,7 @@
         <v>71</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>